<commit_message>
Designed a class tree (not final).
</commit_message>
<xml_diff>
--- a/Ingredients List.xlsx
+++ b/Ingredients List.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\stili\source\repos\Aletta's Kitchen\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{708DF9CD-4BC2-4149-8E38-3A314E7373EA}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C8E525A6-77FB-4FFD-AD0D-9D8F60548B60}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="233" uniqueCount="150">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="234" uniqueCount="151">
   <si>
     <t>Name</t>
   </si>
@@ -202,9 +202,6 @@
   </si>
   <si>
     <t>Big Mac</t>
-  </si>
-  <si>
-    <t>When picked, replace a random ingredient in your kitchen into a 1-point Small Fry</t>
   </si>
   <si>
     <t>Box of Chocolates</t>
@@ -537,6 +534,12 @@
   </si>
   <si>
     <t>Whenever you add 5 or more points to your total Score while this is in the kitchen, gain +5.</t>
+  </si>
+  <si>
+    <t>Rest of Game</t>
+  </si>
+  <si>
+    <t>When picked, replace a random ingredient in your kitchen with a 1-point Small Fry</t>
   </si>
 </sst>
 </file>
@@ -579,7 +582,7 @@
       <charset val="204"/>
     </font>
   </fonts>
-  <fills count="12">
+  <fills count="13">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -646,6 +649,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="3">
     <border>
@@ -681,7 +690,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="31">
+  <cellXfs count="32">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
@@ -727,11 +736,89 @@
     <xf numFmtId="0" fontId="0" fillId="11" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="10" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="34">
+  <dxfs count="45">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="7"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="6"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="2" tint="-0.14996795556505021"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <fill>
         <patternFill>
@@ -1186,9 +1273,9 @@
   </sheetPr>
   <dimension ref="A1:AC88"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="M33" sqref="M33"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A11" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="O66" sqref="O66"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1"/>
@@ -1215,33 +1302,35 @@
         <v>4</v>
       </c>
       <c r="F1" s="24" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="G1" s="25" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="H1" s="25" t="s">
         <v>9</v>
       </c>
       <c r="I1" s="25" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="J1" s="25" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="K1" s="25" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="L1" s="24" t="s">
+        <v>145</v>
+      </c>
+      <c r="M1" s="24" t="s">
         <v>146</v>
       </c>
-      <c r="M1" s="24" t="s">
+      <c r="N1" s="24" t="s">
         <v>147</v>
       </c>
-      <c r="N1" s="24" t="s">
-        <v>148</v>
-      </c>
-      <c r="O1" s="25"/>
+      <c r="O1" s="24" t="s">
+        <v>149</v>
+      </c>
       <c r="P1" s="25"/>
       <c r="Q1" s="25"/>
       <c r="R1" s="25"/>
@@ -2312,8 +2401,8 @@
       <c r="D29" s="10">
         <v>5</v>
       </c>
-      <c r="E29" s="10" t="s">
-        <v>57</v>
+      <c r="E29" s="30" t="s">
+        <v>150</v>
       </c>
       <c r="F29" s="11">
         <f t="shared" si="0"/>
@@ -2339,7 +2428,7 @@
     </row>
     <row r="30" spans="1:29" ht="12.75">
       <c r="A30" s="10" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B30" s="10" t="s">
         <v>6</v>
@@ -2349,7 +2438,7 @@
         <v>0</v>
       </c>
       <c r="E30" s="10" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="F30" s="11">
         <f t="shared" si="0"/>
@@ -2375,7 +2464,7 @@
     </row>
     <row r="31" spans="1:29" ht="12.75">
       <c r="A31" s="10" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B31" s="10" t="s">
         <v>6</v>
@@ -2385,7 +2474,7 @@
         <v>4</v>
       </c>
       <c r="E31" s="10" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="F31" s="11">
         <f t="shared" si="0"/>
@@ -2419,7 +2508,7 @@
     </row>
     <row r="32" spans="1:29" ht="12.75" hidden="1">
       <c r="A32" s="10" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B32" s="10" t="s">
         <v>6</v>
@@ -2449,19 +2538,19 @@
     </row>
     <row r="33" spans="1:21" ht="12.75">
       <c r="A33" s="10" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B33" s="10" t="s">
         <v>6</v>
       </c>
       <c r="C33" s="10" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="D33" s="10">
         <v>2</v>
       </c>
       <c r="E33" s="10" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="F33" s="11">
         <f t="shared" si="0"/>
@@ -2487,19 +2576,19 @@
     </row>
     <row r="34" spans="1:21" ht="12.75">
       <c r="A34" s="10" t="s">
+        <v>65</v>
+      </c>
+      <c r="B34" s="10" t="s">
         <v>66</v>
       </c>
-      <c r="B34" s="10" t="s">
+      <c r="C34" s="10" t="s">
+        <v>63</v>
+      </c>
+      <c r="D34" s="10">
+        <v>1</v>
+      </c>
+      <c r="E34" s="10" t="s">
         <v>67</v>
-      </c>
-      <c r="C34" s="10" t="s">
-        <v>64</v>
-      </c>
-      <c r="D34" s="10">
-        <v>1</v>
-      </c>
-      <c r="E34" s="10" t="s">
-        <v>68</v>
       </c>
       <c r="F34" s="11">
         <f t="shared" si="0"/>
@@ -2525,17 +2614,17 @@
     </row>
     <row r="35" spans="1:21" ht="12.75">
       <c r="A35" s="10" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B35" s="10" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C35" s="11"/>
       <c r="D35" s="10">
         <v>2</v>
       </c>
       <c r="E35" s="10" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="F35" s="11">
         <f t="shared" si="0"/>
@@ -2561,17 +2650,17 @@
     </row>
     <row r="36" spans="1:21" ht="12.75">
       <c r="A36" s="10" t="s">
+        <v>70</v>
+      </c>
+      <c r="B36" s="10" t="s">
         <v>71</v>
-      </c>
-      <c r="B36" s="10" t="s">
-        <v>72</v>
       </c>
       <c r="C36" s="11"/>
       <c r="D36" s="10">
         <v>2</v>
       </c>
       <c r="E36" s="10" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="F36" s="11">
         <f t="shared" si="0"/>
@@ -2597,17 +2686,17 @@
     </row>
     <row r="37" spans="1:21" ht="12.75">
       <c r="A37" s="10" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B37" s="10" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C37" s="11"/>
       <c r="D37" s="10">
         <v>5</v>
       </c>
       <c r="E37" s="30" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="F37" s="11">
         <f t="shared" si="0"/>
@@ -2633,17 +2722,17 @@
     </row>
     <row r="38" spans="1:21" ht="12.75">
       <c r="A38" s="10" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B38" s="10" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C38" s="11"/>
       <c r="D38" s="10">
         <v>1</v>
       </c>
       <c r="E38" s="10" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="F38" s="11">
         <f t="shared" si="0"/>
@@ -2669,7 +2758,7 @@
     </row>
     <row r="39" spans="1:21" ht="12.75" hidden="1">
       <c r="A39" s="10" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B39" s="11"/>
       <c r="C39" s="11"/>
@@ -2697,7 +2786,7 @@
     </row>
     <row r="40" spans="1:21" ht="12.75" hidden="1">
       <c r="A40" s="10" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B40" s="11"/>
       <c r="C40" s="11"/>
@@ -2725,7 +2814,7 @@
     </row>
     <row r="41" spans="1:21" ht="12.75" hidden="1">
       <c r="A41" s="10" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B41" s="11"/>
       <c r="C41" s="11"/>
@@ -2753,7 +2842,7 @@
     </row>
     <row r="42" spans="1:21" ht="12.75">
       <c r="A42" s="10" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B42" s="10" t="s">
         <v>15</v>
@@ -2763,7 +2852,7 @@
         <v>2</v>
       </c>
       <c r="E42" s="10" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="F42" s="11">
         <f t="shared" si="0"/>
@@ -2789,7 +2878,7 @@
     </row>
     <row r="43" spans="1:21" ht="12.75" hidden="1">
       <c r="A43" s="10" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B43" s="10" t="s">
         <v>6</v>
@@ -2819,7 +2908,7 @@
     </row>
     <row r="44" spans="1:21" ht="12.75" hidden="1">
       <c r="A44" s="10" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B44" s="11"/>
       <c r="C44" s="11"/>
@@ -2847,19 +2936,19 @@
     </row>
     <row r="45" spans="1:21" ht="12.75">
       <c r="A45" s="10" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B45" s="10" t="s">
         <v>6</v>
       </c>
       <c r="C45" s="10" t="s">
+        <v>84</v>
+      </c>
+      <c r="D45" s="10">
+        <v>1</v>
+      </c>
+      <c r="E45" s="10" t="s">
         <v>85</v>
-      </c>
-      <c r="D45" s="10">
-        <v>1</v>
-      </c>
-      <c r="E45" s="10" t="s">
-        <v>86</v>
       </c>
       <c r="F45" s="11">
         <f t="shared" si="0"/>
@@ -2885,7 +2974,7 @@
     </row>
     <row r="46" spans="1:21" ht="12.75">
       <c r="A46" s="10" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B46" s="10" t="s">
         <v>6</v>
@@ -2895,11 +2984,11 @@
         <v>1</v>
       </c>
       <c r="E46" s="10" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="F46" s="11">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G46" s="20"/>
       <c r="H46" s="20"/>
@@ -2911,7 +3000,9 @@
       <c r="L46" s="11"/>
       <c r="M46" s="11"/>
       <c r="N46" s="11"/>
-      <c r="O46" s="11"/>
+      <c r="O46" s="11">
+        <v>1</v>
+      </c>
       <c r="P46" s="11"/>
       <c r="Q46" s="11"/>
       <c r="R46" s="11"/>
@@ -2921,19 +3012,19 @@
     </row>
     <row r="47" spans="1:21" ht="12.75">
       <c r="A47" s="10" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B47" s="10" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C47" s="10" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="D47" s="10">
         <v>2</v>
       </c>
       <c r="E47" s="10" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="F47" s="11">
         <f t="shared" si="0"/>
@@ -2959,17 +3050,17 @@
     </row>
     <row r="48" spans="1:21" ht="12.75">
       <c r="A48" s="10" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B48" s="10" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C48" s="11"/>
       <c r="D48" s="10">
         <v>2</v>
       </c>
       <c r="E48" s="10" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="F48" s="11">
         <f t="shared" si="0"/>
@@ -2995,17 +3086,17 @@
     </row>
     <row r="49" spans="1:21" ht="12.75">
       <c r="A49" s="10" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B49" s="10" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C49" s="11"/>
       <c r="D49" s="10">
         <v>1</v>
       </c>
       <c r="E49" s="10" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="F49" s="11">
         <f t="shared" si="0"/>
@@ -3031,17 +3122,17 @@
     </row>
     <row r="50" spans="1:21" ht="12.75">
       <c r="A50" s="10" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B50" s="10" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C50" s="11"/>
       <c r="D50" s="10">
         <v>1</v>
       </c>
       <c r="E50" s="10" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="F50" s="11">
         <f t="shared" si="0"/>
@@ -3067,19 +3158,19 @@
     </row>
     <row r="51" spans="1:21" ht="12.75">
       <c r="A51" s="10" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B51" s="10" t="s">
         <v>15</v>
       </c>
       <c r="C51" s="10" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="D51" s="10">
         <v>10</v>
       </c>
       <c r="E51" s="10" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="F51" s="11">
         <f t="shared" si="0"/>
@@ -3105,7 +3196,7 @@
     </row>
     <row r="52" spans="1:21" ht="12.75" hidden="1">
       <c r="A52" s="10" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B52" s="11"/>
       <c r="C52" s="11"/>
@@ -3133,7 +3224,7 @@
     </row>
     <row r="53" spans="1:21" ht="12.75" hidden="1">
       <c r="A53" s="10" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B53" s="11"/>
       <c r="C53" s="11"/>
@@ -3161,7 +3252,7 @@
     </row>
     <row r="54" spans="1:21" ht="12.75" hidden="1">
       <c r="A54" s="10" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B54" s="11"/>
       <c r="C54" s="11"/>
@@ -3189,10 +3280,10 @@
     </row>
     <row r="55" spans="1:21" ht="12.75" hidden="1">
       <c r="A55" s="10" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="B55" s="10" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C55" s="11"/>
       <c r="D55" s="11"/>
@@ -3219,7 +3310,7 @@
     </row>
     <row r="56" spans="1:21" ht="12.75" hidden="1">
       <c r="A56" s="10" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B56" s="11"/>
       <c r="C56" s="11"/>
@@ -3247,7 +3338,7 @@
     </row>
     <row r="57" spans="1:21" ht="12.75" hidden="1">
       <c r="A57" s="10" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B57" s="11"/>
       <c r="C57" s="11"/>
@@ -3275,17 +3366,17 @@
     </row>
     <row r="58" spans="1:21" ht="12.75">
       <c r="A58" s="10" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="B58" s="10" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C58" s="11"/>
       <c r="D58" s="10">
         <v>3</v>
       </c>
       <c r="E58" s="10" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="F58" s="11">
         <f t="shared" si="0"/>
@@ -3311,7 +3402,7 @@
     </row>
     <row r="59" spans="1:21" ht="12.75">
       <c r="A59" s="10" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="B59" s="10" t="s">
         <v>6</v>
@@ -3345,17 +3436,17 @@
     </row>
     <row r="60" spans="1:21" ht="12.75">
       <c r="A60" s="10" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="B60" s="10" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C60" s="11"/>
       <c r="D60" s="10">
         <v>2</v>
       </c>
       <c r="E60" s="10" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="F60" s="11">
         <f t="shared" si="0"/>
@@ -3381,7 +3472,7 @@
     </row>
     <row r="61" spans="1:21" ht="12.75">
       <c r="A61" s="10" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="B61" s="10" t="s">
         <v>15</v>
@@ -3391,7 +3482,7 @@
         <v>2</v>
       </c>
       <c r="E61" s="10" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="F61" s="11">
         <f t="shared" si="0"/>
@@ -3415,15 +3506,15 @@
     </row>
     <row r="62" spans="1:21" ht="12.75">
       <c r="A62" s="10" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="B62" s="10" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C62" s="11"/>
       <c r="D62" s="11"/>
       <c r="E62" s="10" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="F62" s="11">
         <f t="shared" si="0"/>
@@ -3447,7 +3538,7 @@
     </row>
     <row r="63" spans="1:21" ht="12.75">
       <c r="A63" s="10" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="B63" s="10" t="s">
         <v>15</v>
@@ -3459,7 +3550,7 @@
         <v>0</v>
       </c>
       <c r="E63" s="10" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="F63" s="11">
         <f t="shared" si="0"/>
@@ -3485,7 +3576,7 @@
     </row>
     <row r="64" spans="1:21" ht="12.75">
       <c r="A64" s="10" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="B64" s="10" t="s">
         <v>15</v>
@@ -3497,11 +3588,11 @@
         <v>5</v>
       </c>
       <c r="E64" s="10" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="F64" s="11">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G64" s="20"/>
       <c r="H64" s="20"/>
@@ -3513,7 +3604,9 @@
       <c r="L64" s="11"/>
       <c r="M64" s="11"/>
       <c r="N64" s="11"/>
-      <c r="O64" s="11"/>
+      <c r="O64" s="11">
+        <v>1</v>
+      </c>
       <c r="P64" s="11"/>
       <c r="Q64" s="11"/>
       <c r="R64" s="11"/>
@@ -3523,7 +3616,7 @@
     </row>
     <row r="65" spans="1:21" ht="12.75">
       <c r="A65" s="10" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="B65" s="10" t="s">
         <v>15</v>
@@ -3533,7 +3626,7 @@
         <v>9</v>
       </c>
       <c r="E65" s="10" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="F65" s="11">
         <f t="shared" si="0"/>
@@ -3566,7 +3659,7 @@
       <c r="L66" s="27"/>
       <c r="M66" s="28"/>
       <c r="N66" s="29"/>
-      <c r="O66" s="11"/>
+      <c r="O66" s="31"/>
       <c r="P66" s="11"/>
       <c r="Q66" s="11"/>
       <c r="R66" s="11"/>
@@ -3576,53 +3669,53 @@
     </row>
     <row r="67" spans="1:21" ht="12.75" hidden="1">
       <c r="A67" s="4" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
     <row r="68" spans="1:21" ht="12.75" hidden="1">
       <c r="A68" s="4" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="69" spans="1:21" ht="12.75" hidden="1">
       <c r="A69" s="4" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
     <row r="70" spans="1:21" ht="12.75" hidden="1">
       <c r="A70" s="4" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
     </row>
     <row r="71" spans="1:21" ht="12.75" hidden="1">
       <c r="A71" s="4" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
     </row>
     <row r="72" spans="1:21" ht="12.75" hidden="1">
       <c r="A72" s="4" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
     </row>
     <row r="73" spans="1:21" ht="12.75" hidden="1">
       <c r="A73" s="4" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
     </row>
     <row r="74" spans="1:21" ht="12.75" hidden="1">
       <c r="A74" s="4" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
     <row r="75" spans="1:21" ht="12.75" hidden="1">
       <c r="A75" s="4" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
     </row>
     <row r="76" spans="1:21" ht="12.75" hidden="1"/>
     <row r="77" spans="1:21" ht="12.75" hidden="1">
       <c r="A77" s="4" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="C77" s="4" t="s">
         <v>18</v>
@@ -3631,7 +3724,7 @@
     </row>
     <row r="78" spans="1:21" ht="12.75" hidden="1">
       <c r="A78" s="4" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="C78" s="4" t="s">
         <v>18</v>
@@ -3640,12 +3733,12 @@
     </row>
     <row r="79" spans="1:21" ht="12.75" hidden="1">
       <c r="A79" s="4" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
     <row r="80" spans="1:21" ht="12.75" hidden="1">
       <c r="A80" s="4" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="B80" s="4" t="s">
         <v>15</v>
@@ -3657,24 +3750,24 @@
     </row>
     <row r="81" spans="1:29" ht="12.75" hidden="1">
       <c r="A81" s="4" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="B81" s="4" t="s">
         <v>15</v>
       </c>
       <c r="E81" s="4" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
     </row>
     <row r="82" spans="1:29" ht="12.75" hidden="1">
       <c r="A82" s="4" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="B82" s="4" t="s">
         <v>15</v>
       </c>
       <c r="E82" s="4" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
     </row>
     <row r="83" spans="1:29" ht="12.75" hidden="1">
@@ -3682,12 +3775,12 @@
         <v>15</v>
       </c>
       <c r="E83" s="4" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
     </row>
     <row r="84" spans="1:29" ht="12.75" hidden="1">
       <c r="A84" s="7" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="B84" s="7" t="s">
         <v>15</v>
@@ -3695,7 +3788,7 @@
       <c r="C84" s="6"/>
       <c r="D84" s="6"/>
       <c r="E84" s="9" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="F84" s="6"/>
       <c r="G84" s="6"/>
@@ -3724,7 +3817,7 @@
     </row>
     <row r="85" spans="1:29" ht="12.75" hidden="1">
       <c r="A85" s="4" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="B85" s="4" t="s">
         <v>15</v>
@@ -3738,7 +3831,7 @@
       <c r="C86" s="8"/>
       <c r="D86" s="8"/>
       <c r="E86" s="5" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="F86" s="6"/>
       <c r="G86" s="6"/>
@@ -3768,60 +3861,65 @@
     <row r="87" spans="1:29" ht="12.75" hidden="1"/>
     <row r="88" spans="1:29" ht="12.75" hidden="1">
       <c r="A88" s="4" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="B88" s="4" t="s">
         <v>15</v>
       </c>
       <c r="E88" s="4" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
   </sheetData>
   <conditionalFormatting sqref="G2:G65">
-    <cfRule type="cellIs" dxfId="18" priority="10" operator="equal">
+    <cfRule type="cellIs" dxfId="20" priority="11" operator="equal">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H2:H65">
-    <cfRule type="cellIs" dxfId="17" priority="9" operator="equal">
+    <cfRule type="cellIs" dxfId="19" priority="10" operator="equal">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I2:I65">
-    <cfRule type="cellIs" dxfId="16" priority="8" operator="equal">
+    <cfRule type="cellIs" dxfId="18" priority="9" operator="equal">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J2:J65">
-    <cfRule type="cellIs" dxfId="15" priority="7" operator="equal">
+    <cfRule type="cellIs" dxfId="17" priority="8" operator="equal">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K2:K65">
-    <cfRule type="cellIs" dxfId="14" priority="6" operator="equal">
+    <cfRule type="cellIs" dxfId="16" priority="7" operator="equal">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F2:F65">
-    <cfRule type="cellIs" dxfId="13" priority="5" stopIfTrue="1" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="15" priority="6" stopIfTrue="1" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
-    <cfRule type="notContainsErrors" dxfId="12" priority="10">
+    <cfRule type="notContainsErrors" dxfId="14" priority="11">
       <formula>NOT(ISERROR(F2))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L2:L65">
-    <cfRule type="cellIs" dxfId="11" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="13" priority="4" operator="equal">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N2:N65">
-    <cfRule type="cellIs" dxfId="10" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="12" priority="3" operator="equal">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M2:M65">
+    <cfRule type="cellIs" dxfId="11" priority="2" operator="equal">
+      <formula>1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="O2:O65">
     <cfRule type="cellIs" dxfId="0" priority="1" operator="equal">
       <formula>1</formula>
     </cfRule>

</xml_diff>